<commit_message>
[pdq] aggiornato test e grafico test di sistema
</commit_message>
<xml_diff>
--- a/PianoDiQualifica/Img/Excel/Resoconto_Test.xlsx
+++ b/PianoDiQualifica/Img/Excel/Resoconto_Test.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Desktop\7DOS\7DOS\PianoDiQualifica\Img\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TI" sheetId="1" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="TS" sheetId="3" r:id="rId3"/>
     <sheet name="TA" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -110,9 +105,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -170,26 +165,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -215,7 +190,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-0D1D-4689-BB81-A779F8EC9F95}"/>
               </c:ext>
@@ -235,7 +210,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-0D1D-4689-BB81-A779F8EC9F95}"/>
               </c:ext>
@@ -255,7 +230,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-0D1D-4689-BB81-A779F8EC9F95}"/>
               </c:ext>
@@ -275,7 +250,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-0D1D-4689-BB81-A779F8EC9F95}"/>
               </c:ext>
@@ -285,7 +260,7 @@
             <c:dLbl>
               <c:idx val="0"/>
               <c:delete val="1"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-0D1D-4689-BB81-A779F8EC9F95}"/>
@@ -295,7 +270,7 @@
             <c:dLbl>
               <c:idx val="1"/>
               <c:delete val="1"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-0D1D-4689-BB81-A779F8EC9F95}"/>
@@ -305,7 +280,7 @@
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-0D1D-4689-BB81-A779F8EC9F95}"/>
@@ -335,7 +310,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
@@ -378,7 +353,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -389,7 +364,7 @@
             <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <a:prstGeom prst="wedgeRectCallout">
@@ -444,7 +419,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0D1D-4689-BB81-A779F8EC9F95}"/>
             </c:ext>
@@ -506,7 +481,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -536,7 +511,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -548,9 +523,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -603,26 +578,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -648,7 +603,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-B4D9-40AC-B864-4799C86B25F3}"/>
               </c:ext>
@@ -668,7 +623,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-B4D9-40AC-B864-4799C86B25F3}"/>
               </c:ext>
@@ -688,7 +643,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-B4D9-40AC-B864-4799C86B25F3}"/>
               </c:ext>
@@ -708,7 +663,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-B4D9-40AC-B864-4799C86B25F3}"/>
               </c:ext>
@@ -718,7 +673,7 @@
             <c:dLbl>
               <c:idx val="0"/>
               <c:delete val="1"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
@@ -730,7 +685,7 @@
             <c:dLbl>
               <c:idx val="1"/>
               <c:delete val="1"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-B4D9-40AC-B864-4799C86B25F3}"/>
@@ -740,7 +695,7 @@
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-B4D9-40AC-B864-4799C86B25F3}"/>
@@ -780,7 +735,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -791,7 +746,7 @@
             <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <a:prstGeom prst="wedgeRectCallout">
@@ -847,7 +802,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B4D9-40AC-B864-4799C86B25F3}"/>
             </c:ext>
@@ -900,7 +855,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -930,7 +885,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -942,9 +897,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1002,26 +957,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1047,7 +982,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-A8C2-49B8-8092-49B26948B3F9}"/>
               </c:ext>
@@ -1067,7 +1002,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-A8C2-49B8-8092-49B26948B3F9}"/>
               </c:ext>
@@ -1087,7 +1022,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-A8C2-49B8-8092-49B26948B3F9}"/>
               </c:ext>
@@ -1107,7 +1042,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-A8C2-49B8-8092-49B26948B3F9}"/>
               </c:ext>
@@ -1115,44 +1050,9 @@
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{AA1E16FC-ACC6-476F-8C79-4FCD616AF074}" type="PERCENTAGE">
-                      <a:rPr lang="en-US" sz="1100" baseline="0"/>
-                      <a:pPr/>
-                      <a:t>[PERCENTUALE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="it-IT"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="0"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-A8C2-49B8-8092-49B26948B3F9}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
               <c:idx val="1"/>
               <c:delete val="1"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-A8C2-49B8-8092-49B26948B3F9}"/>
@@ -1162,45 +1062,10 @@
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-A8C2-49B8-8092-49B26948B3F9}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{C5264198-FE66-46F7-B4BE-628490FDE5AD}" type="PERCENTAGE">
-                      <a:rPr lang="en-US" sz="1100" baseline="0"/>
-                      <a:pPr/>
-                      <a:t>[PERCENTUALE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="it-IT"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="0"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-A8C2-49B8-8092-49B26948B3F9}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1237,7 +1102,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1248,7 +1113,7 @@
             <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <a:prstGeom prst="wedgeRectCallout">
@@ -1289,7 +1154,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1303,7 +1168,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-A8C2-49B8-8092-49B26948B3F9}"/>
             </c:ext>
@@ -1356,7 +1221,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1386,7 +1251,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1398,9 +1263,9 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1458,26 +1323,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1503,7 +1348,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-7186-4BDA-8750-47245A588A5B}"/>
               </c:ext>
@@ -1523,7 +1368,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-7186-4BDA-8750-47245A588A5B}"/>
               </c:ext>
@@ -1543,7 +1388,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-7186-4BDA-8750-47245A588A5B}"/>
               </c:ext>
@@ -1563,7 +1408,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-7186-4BDA-8750-47245A588A5B}"/>
               </c:ext>
@@ -1593,7 +1438,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
@@ -1626,7 +1471,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
@@ -1659,7 +1504,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
@@ -1692,7 +1537,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
@@ -1735,7 +1580,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1746,7 +1591,7 @@
             <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <a:prstGeom prst="wedgeRectCallout">
@@ -1801,7 +1646,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-7186-4BDA-8750-47245A588A5B}"/>
             </c:ext>
@@ -1853,7 +1698,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1883,7 +1728,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4529,7 +4374,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4543,15 +4388,15 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4565,7 +4410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0</v>
       </c>
@@ -4589,20 +4434,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4616,7 +4461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0</v>
       </c>
@@ -4640,19 +4485,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:F3"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:6" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="3:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4666,9 +4511,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C3">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -4694,15 +4539,15 @@
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:6" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="3:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4716,7 +4561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>25</v>
       </c>

</xml_diff>